<commit_message>
Try to configure fb. Not working
</commit_message>
<xml_diff>
--- a/db/seeds_databases/washers_db.xlsx
+++ b/db/seeds_databases/washers_db.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/medularis/Library/Containers/com.microsoft.Excel/Data/Desktop/DesafioLatam/50-Parkwash/parkwash_rails_v2/db/seeds_databases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Desktop/Proyectos-Rails/parkwash/parkwash3/db/seeds_databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DCF2A8-AC61-1F4A-AA8B-45C1D4F30156}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{993CAC9A-2043-DC48-A9CB-701634364864}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>rut</t>
   </si>
@@ -43,9 +48,6 @@
   </si>
   <si>
     <t>city</t>
-  </si>
-  <si>
-    <t>birth_date</t>
   </si>
   <si>
     <t>role</t>
@@ -117,10 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy;@"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -150,9 +149,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,11 +464,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D77A8A-279A-674B-8F38-7246BD7BF0E5}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +476,7 @@
     <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,163 +498,142 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2">
         <v>56935394641</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1">
-        <v>36526</v>
-      </c>
-      <c r="H2">
+        <v>11</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1">
-        <v>36526</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1">
-        <v>36526</v>
-      </c>
-      <c r="H4">
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1">
-        <v>36526</v>
-      </c>
-      <c r="H5">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1">
-        <v>36526</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1">
-        <v>36526</v>
-      </c>
-      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
     </row>

</xml_diff>